<commit_message>
vault backup: 2025-05-26 09:03:57
</commit_message>
<xml_diff>
--- a/Planning de Estudio OSCP.xlsx
+++ b/Planning de Estudio OSCP.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://enerclic-my.sharepoint.com/personal/aprieto_enerclic_es/Documents/Escritorio/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://enerclic-my.sharepoint.com/personal/aprieto_enerclic_es/Documents/Escritorio/PNPT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="11_8950C97D1B3218331BB8EA49AB1BDE76198F71D2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4ED03042-2FB7-48DC-B4BC-451405A0FDB8}"/>
+  <xr:revisionPtr revIDLastSave="64" documentId="11_8950C97D1B3218331BB8EA49AB1BDE76198F71D2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{62717F14-E0A8-409E-BE85-146FBF9AEB3C}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HackTheBox" sheetId="1" r:id="rId1"/>
@@ -8250,7 +8250,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -8384,26 +8384,32 @@
     <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -8626,34 +8632,34 @@
   </sheetPr>
   <dimension ref="A2:H302"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E205" workbookViewId="0">
-      <selection activeCell="G225" sqref="G225"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
     <col min="5" max="5" width="86" customWidth="1"/>
-    <col min="6" max="6" width="33.6640625" customWidth="1"/>
+    <col min="6" max="6" width="33.7109375" customWidth="1"/>
     <col min="7" max="7" width="44" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
+    <row r="2" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="51"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="52"/>
       <c r="E2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -8679,7 +8685,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
@@ -8705,7 +8711,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
@@ -8731,7 +8737,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>24</v>
       </c>
@@ -8757,7 +8763,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>30</v>
       </c>
@@ -8783,7 +8789,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>35</v>
       </c>
@@ -8809,7 +8815,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>41</v>
       </c>
@@ -8835,7 +8841,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>46</v>
       </c>
@@ -8861,7 +8867,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>51</v>
       </c>
@@ -8887,7 +8893,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>57</v>
       </c>
@@ -8913,7 +8919,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>62</v>
       </c>
@@ -8939,7 +8945,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>67</v>
       </c>
@@ -8965,7 +8971,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>72</v>
       </c>
@@ -8991,7 +8997,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>77</v>
       </c>
@@ -9017,7 +9023,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>82</v>
       </c>
@@ -9030,7 +9036,7 @@
       <c r="D18" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="60" t="s">
+      <c r="E18" s="49" t="s">
         <v>84</v>
       </c>
       <c r="F18" s="8" t="s">
@@ -9040,10 +9046,10 @@
         <v>86</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>1627</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>87</v>
       </c>
@@ -9069,7 +9075,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>91</v>
       </c>
@@ -9095,7 +9101,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>95</v>
       </c>
@@ -9121,7 +9127,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>100</v>
       </c>
@@ -9134,10 +9140,10 @@
       <c r="D22" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="E22" s="49" t="s">
         <v>102</v>
       </c>
-      <c r="F22" s="8" t="s">
+      <c r="F22" s="61" t="s">
         <v>103</v>
       </c>
       <c r="G22" s="13" t="s">
@@ -9147,7 +9153,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>105</v>
       </c>
@@ -9173,7 +9179,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>109</v>
       </c>
@@ -9199,7 +9205,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>114</v>
       </c>
@@ -9225,7 +9231,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>118</v>
       </c>
@@ -9251,7 +9257,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>123</v>
       </c>
@@ -9267,7 +9273,7 @@
       <c r="E27" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="F27" s="8" t="s">
+      <c r="F27" s="61" t="s">
         <v>126</v>
       </c>
       <c r="G27" s="13" t="s">
@@ -9277,7 +9283,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>128</v>
       </c>
@@ -9303,7 +9309,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>133</v>
       </c>
@@ -9326,10 +9332,10 @@
         <v>136</v>
       </c>
       <c r="H29" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1627</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>137</v>
       </c>
@@ -9345,7 +9351,7 @@
       <c r="E30" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="F30" s="8" t="s">
+      <c r="F30" s="61" t="s">
         <v>140</v>
       </c>
       <c r="G30" s="9" t="s">
@@ -9355,7 +9361,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>142</v>
       </c>
@@ -9381,7 +9387,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>147</v>
       </c>
@@ -9407,7 +9413,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>151</v>
       </c>
@@ -9433,7 +9439,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>155</v>
       </c>
@@ -9459,7 +9465,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>160</v>
       </c>
@@ -9485,7 +9491,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>165</v>
       </c>
@@ -9511,7 +9517,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>170</v>
       </c>
@@ -9537,7 +9543,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>175</v>
       </c>
@@ -9563,7 +9569,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>179</v>
       </c>
@@ -9589,7 +9595,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>183</v>
       </c>
@@ -9615,7 +9621,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>188</v>
       </c>
@@ -9641,7 +9647,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>192</v>
       </c>
@@ -9667,7 +9673,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>197</v>
       </c>
@@ -9693,7 +9699,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>201</v>
       </c>
@@ -9719,7 +9725,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>206</v>
       </c>
@@ -9745,7 +9751,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>210</v>
       </c>
@@ -9771,7 +9777,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>215</v>
       </c>
@@ -9797,7 +9803,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>220</v>
       </c>
@@ -9823,7 +9829,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>224</v>
       </c>
@@ -9849,7 +9855,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>229</v>
       </c>
@@ -9875,7 +9881,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>233</v>
       </c>
@@ -9901,7 +9907,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>238</v>
       </c>
@@ -9917,7 +9923,7 @@
       <c r="E52" s="7" t="s">
         <v>240</v>
       </c>
-      <c r="F52" s="8" t="s">
+      <c r="F52" s="61" t="s">
         <v>213</v>
       </c>
       <c r="G52" s="16" t="s">
@@ -9927,7 +9933,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>242</v>
       </c>
@@ -9953,7 +9959,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>247</v>
       </c>
@@ -9979,7 +9985,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>251</v>
       </c>
@@ -10005,7 +10011,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>255</v>
       </c>
@@ -10031,7 +10037,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>259</v>
       </c>
@@ -10057,7 +10063,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>264</v>
       </c>
@@ -10083,7 +10089,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>268</v>
       </c>
@@ -10099,7 +10105,7 @@
       <c r="E59" s="7" t="s">
         <v>270</v>
       </c>
-      <c r="F59" s="8" t="s">
+      <c r="F59" s="61" t="s">
         <v>271</v>
       </c>
       <c r="G59" s="16" t="s">
@@ -10109,7 +10115,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>273</v>
       </c>
@@ -10135,7 +10141,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>277</v>
       </c>
@@ -10161,7 +10167,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>282</v>
       </c>
@@ -10184,10 +10190,10 @@
         <v>286</v>
       </c>
       <c r="H62" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1627</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>287</v>
       </c>
@@ -10203,7 +10209,7 @@
       <c r="E63" s="7" t="s">
         <v>289</v>
       </c>
-      <c r="F63" s="8" t="s">
+      <c r="F63" s="61" t="s">
         <v>290</v>
       </c>
       <c r="G63" s="9" t="s">
@@ -10213,7 +10219,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>292</v>
       </c>
@@ -10239,7 +10245,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>297</v>
       </c>
@@ -10265,7 +10271,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="66" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
         <v>302</v>
       </c>
@@ -10291,7 +10297,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="67" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
         <v>307</v>
       </c>
@@ -10317,7 +10323,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
         <v>311</v>
       </c>
@@ -10343,7 +10349,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="69" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
         <v>316</v>
       </c>
@@ -10369,7 +10375,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="70" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
         <v>321</v>
       </c>
@@ -10395,7 +10401,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="71" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>326</v>
       </c>
@@ -10421,7 +10427,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="72" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
         <v>330</v>
       </c>
@@ -10447,7 +10453,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
         <v>335</v>
       </c>
@@ -10463,7 +10469,7 @@
       <c r="E73" s="7" t="s">
         <v>337</v>
       </c>
-      <c r="F73" s="8" t="s">
+      <c r="F73" s="61" t="s">
         <v>338</v>
       </c>
       <c r="G73" s="9" t="s">
@@ -10473,7 +10479,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
         <v>340</v>
       </c>
@@ -10499,7 +10505,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="75" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
         <v>345</v>
       </c>
@@ -10525,7 +10531,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
         <v>350</v>
       </c>
@@ -10551,7 +10557,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
         <v>354</v>
       </c>
@@ -10577,7 +10583,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="78" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
         <v>358</v>
       </c>
@@ -10603,7 +10609,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="79" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
         <v>362</v>
       </c>
@@ -10629,7 +10635,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="80" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
         <v>366</v>
       </c>
@@ -10655,7 +10661,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
         <v>371</v>
       </c>
@@ -10681,7 +10687,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
         <v>375</v>
       </c>
@@ -10697,7 +10703,7 @@
       <c r="E82" s="7" t="s">
         <v>377</v>
       </c>
-      <c r="F82" s="8" t="s">
+      <c r="F82" s="61" t="s">
         <v>295</v>
       </c>
       <c r="G82" s="16" t="s">
@@ -10707,7 +10713,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
         <v>379</v>
       </c>
@@ -10733,7 +10739,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="84" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
         <v>383</v>
       </c>
@@ -10759,7 +10765,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
         <v>388</v>
       </c>
@@ -10785,7 +10791,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="86" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
         <v>392</v>
       </c>
@@ -10811,7 +10817,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
         <v>396</v>
       </c>
@@ -10827,7 +10833,7 @@
       <c r="E87" s="7" t="s">
         <v>398</v>
       </c>
-      <c r="F87" s="8" t="s">
+      <c r="F87" s="61" t="s">
         <v>186</v>
       </c>
       <c r="G87" s="9" t="s">
@@ -10837,7 +10843,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
         <v>400</v>
       </c>
@@ -10863,7 +10869,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
         <v>404</v>
       </c>
@@ -10889,7 +10895,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
         <v>408</v>
       </c>
@@ -10915,7 +10921,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
         <v>412</v>
       </c>
@@ -10931,7 +10937,7 @@
       <c r="E91" s="7" t="s">
         <v>414</v>
       </c>
-      <c r="F91" s="8" t="s">
+      <c r="F91" s="61" t="s">
         <v>415</v>
       </c>
       <c r="G91" s="9" t="s">
@@ -10941,7 +10947,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
         <v>417</v>
       </c>
@@ -10967,7 +10973,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
         <v>421</v>
       </c>
@@ -10993,7 +10999,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
         <v>425</v>
       </c>
@@ -11019,7 +11025,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
         <v>430</v>
       </c>
@@ -11045,7 +11051,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="79.2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
         <v>434</v>
       </c>
@@ -11058,10 +11064,10 @@
       <c r="D96" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E96" s="60" t="s">
+      <c r="E96" s="49" t="s">
         <v>436</v>
       </c>
-      <c r="F96" s="8" t="s">
+      <c r="F96" s="61" t="s">
         <v>65</v>
       </c>
       <c r="G96" s="9" t="s">
@@ -11071,7 +11077,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="97" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
         <v>438</v>
       </c>
@@ -11097,7 +11103,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="98" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
         <v>442</v>
       </c>
@@ -11123,7 +11129,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="99" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
         <v>447</v>
       </c>
@@ -11149,7 +11155,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="100" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
         <v>452</v>
       </c>
@@ -11175,7 +11181,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="101" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
         <v>456</v>
       </c>
@@ -11201,7 +11207,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="102" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
         <v>460</v>
       </c>
@@ -11227,7 +11233,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
         <v>464</v>
       </c>
@@ -11243,7 +11249,7 @@
       <c r="E103" s="7" t="s">
         <v>466</v>
       </c>
-      <c r="F103" s="8" t="s">
+      <c r="F103" s="61" t="s">
         <v>295</v>
       </c>
       <c r="G103" s="9" t="s">
@@ -11253,7 +11259,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="104" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
         <v>468</v>
       </c>
@@ -11279,7 +11285,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="105" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
         <v>472</v>
       </c>
@@ -11305,7 +11311,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="106" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
         <v>476</v>
       </c>
@@ -11331,7 +11337,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="107" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
         <v>480</v>
       </c>
@@ -11357,7 +11363,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
         <v>484</v>
       </c>
@@ -11373,7 +11379,7 @@
       <c r="E108" s="7" t="s">
         <v>486</v>
       </c>
-      <c r="F108" s="8" t="s">
+      <c r="F108" s="61" t="s">
         <v>295</v>
       </c>
       <c r="G108" s="9" t="s">
@@ -11383,7 +11389,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="109" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
         <v>488</v>
       </c>
@@ -11409,7 +11415,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="110" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
         <v>492</v>
       </c>
@@ -11435,7 +11441,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="111" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
         <v>496</v>
       </c>
@@ -11461,7 +11467,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="112" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
         <v>500</v>
       </c>
@@ -11487,7 +11493,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="113" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
         <v>504</v>
       </c>
@@ -11513,7 +11519,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="114" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
         <v>508</v>
       </c>
@@ -11539,7 +11545,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="115" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
         <v>513</v>
       </c>
@@ -11565,7 +11571,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="116" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
         <v>517</v>
       </c>
@@ -11591,7 +11597,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" s="3" t="s">
         <v>521</v>
       </c>
@@ -11617,7 +11623,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="s">
         <v>526</v>
       </c>
@@ -11643,7 +11649,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="s">
         <v>530</v>
       </c>
@@ -11659,7 +11665,7 @@
       <c r="E119" s="7" t="s">
         <v>532</v>
       </c>
-      <c r="F119" s="8" t="s">
+      <c r="F119" s="61" t="s">
         <v>271</v>
       </c>
       <c r="G119" s="16" t="s">
@@ -11669,7 +11675,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="120" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" s="3" t="s">
         <v>534</v>
       </c>
@@ -11695,7 +11701,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="121" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" s="3" t="s">
         <v>538</v>
       </c>
@@ -11721,7 +11727,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="122" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" s="3" t="s">
         <v>543</v>
       </c>
@@ -11747,7 +11753,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="123" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" s="3" t="s">
         <v>547</v>
       </c>
@@ -11773,7 +11779,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="124" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" s="3" t="s">
         <v>551</v>
       </c>
@@ -11799,7 +11805,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="125" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" s="3" t="s">
         <v>555</v>
       </c>
@@ -11825,7 +11831,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" s="3" t="s">
         <v>560</v>
       </c>
@@ -11851,7 +11857,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A127" s="3" t="s">
         <v>564</v>
       </c>
@@ -11867,7 +11873,7 @@
       <c r="E127" s="7" t="s">
         <v>566</v>
       </c>
-      <c r="F127" s="8" t="s">
+      <c r="F127" s="61" t="s">
         <v>567</v>
       </c>
       <c r="G127" s="16" t="s">
@@ -11877,7 +11883,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="128" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" s="3" t="s">
         <v>569</v>
       </c>
@@ -11903,7 +11909,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A129" s="3" t="s">
         <v>573</v>
       </c>
@@ -11919,7 +11925,7 @@
       <c r="E129" s="7" t="s">
         <v>575</v>
       </c>
-      <c r="F129" s="8" t="s">
+      <c r="F129" s="61" t="s">
         <v>65</v>
       </c>
       <c r="G129" s="16" t="s">
@@ -11929,7 +11935,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="130" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" s="3" t="s">
         <v>577</v>
       </c>
@@ -11955,7 +11961,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="131" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" s="3" t="s">
         <v>581</v>
       </c>
@@ -11981,7 +11987,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="132" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" s="3" t="s">
         <v>586</v>
       </c>
@@ -12007,7 +12013,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="133" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" s="3" t="s">
         <v>590</v>
       </c>
@@ -12033,7 +12039,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A134" s="3" t="s">
         <v>594</v>
       </c>
@@ -12049,7 +12055,7 @@
       <c r="E134" s="7" t="s">
         <v>596</v>
       </c>
-      <c r="F134" s="8" t="s">
+      <c r="F134" s="61" t="s">
         <v>65</v>
       </c>
       <c r="G134" s="16" t="s">
@@ -12059,7 +12065,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="135" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" s="3" t="s">
         <v>598</v>
       </c>
@@ -12085,7 +12091,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="136" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" s="3" t="s">
         <v>603</v>
       </c>
@@ -12111,7 +12117,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="137" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" s="3" t="s">
         <v>608</v>
       </c>
@@ -12137,7 +12143,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="138" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" s="3" t="s">
         <v>613</v>
       </c>
@@ -12163,7 +12169,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="139" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" s="3" t="s">
         <v>617</v>
       </c>
@@ -12189,7 +12195,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="140" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" s="3" t="s">
         <v>621</v>
       </c>
@@ -12215,7 +12221,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="141" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" s="3" t="s">
         <v>625</v>
       </c>
@@ -12241,7 +12247,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A142" s="18" t="s">
         <v>629</v>
       </c>
@@ -12257,7 +12263,7 @@
       <c r="E142" s="20" t="s">
         <v>631</v>
       </c>
-      <c r="F142" s="21" t="s">
+      <c r="F142" s="62" t="s">
         <v>70</v>
       </c>
       <c r="G142" s="16" t="s">
@@ -12267,7 +12273,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="143" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" s="3" t="s">
         <v>633</v>
       </c>
@@ -12293,7 +12299,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="144" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" s="3" t="s">
         <v>637</v>
       </c>
@@ -12319,7 +12325,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="145" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" s="3" t="s">
         <v>641</v>
       </c>
@@ -12345,7 +12351,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A146" s="18" t="s">
         <v>646</v>
       </c>
@@ -12371,7 +12377,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="147" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" s="3" t="s">
         <v>650</v>
       </c>
@@ -12397,7 +12403,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="148" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" s="3" t="s">
         <v>655</v>
       </c>
@@ -12423,7 +12429,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A149" s="18" t="s">
         <v>659</v>
       </c>
@@ -12439,7 +12445,7 @@
       <c r="E149" s="20" t="s">
         <v>661</v>
       </c>
-      <c r="F149" s="21" t="s">
+      <c r="F149" s="62" t="s">
         <v>662</v>
       </c>
       <c r="G149" s="16" t="s">
@@ -12449,7 +12455,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="150" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" s="3" t="s">
         <v>664</v>
       </c>
@@ -12475,7 +12481,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A151" s="18" t="s">
         <v>669</v>
       </c>
@@ -12491,7 +12497,7 @@
       <c r="E151" s="20" t="s">
         <v>671</v>
       </c>
-      <c r="F151" s="21" t="s">
+      <c r="F151" s="62" t="s">
         <v>662</v>
       </c>
       <c r="G151" s="16" t="s">
@@ -12501,7 +12507,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="152" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152" s="3" t="s">
         <v>673</v>
       </c>
@@ -12527,7 +12533,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A153" s="3" t="s">
         <v>677</v>
       </c>
@@ -12543,7 +12549,7 @@
       <c r="E153" s="7" t="s">
         <v>679</v>
       </c>
-      <c r="F153" s="8" t="s">
+      <c r="F153" s="61" t="s">
         <v>295</v>
       </c>
       <c r="G153" s="16" t="s">
@@ -12553,7 +12559,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="154" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154" s="3" t="s">
         <v>681</v>
       </c>
@@ -12579,7 +12585,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="155" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155" s="3" t="s">
         <v>686</v>
       </c>
@@ -12605,7 +12611,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="156" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A156" s="3" t="s">
         <v>691</v>
       </c>
@@ -12631,7 +12637,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="157" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A157" s="3" t="s">
         <v>696</v>
       </c>
@@ -12657,7 +12663,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="158" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A158" s="3" t="s">
         <v>700</v>
       </c>
@@ -12683,7 +12689,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="159" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A159" s="3" t="s">
         <v>705</v>
       </c>
@@ -12709,7 +12715,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A160" s="3" t="s">
         <v>709</v>
       </c>
@@ -12735,7 +12741,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="161" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161" s="3" t="s">
         <v>713</v>
       </c>
@@ -12761,7 +12767,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="162" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162" s="3" t="s">
         <v>717</v>
       </c>
@@ -12787,7 +12793,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A163" s="3" t="s">
         <v>721</v>
       </c>
@@ -12813,7 +12819,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" s="3" t="s">
         <v>725</v>
       </c>
@@ -12839,7 +12845,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="165" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165" s="3" t="s">
         <v>729</v>
       </c>
@@ -12865,7 +12871,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="166" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166" s="3" t="s">
         <v>733</v>
       </c>
@@ -12891,7 +12897,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A167" s="3" t="s">
         <v>737</v>
       </c>
@@ -12907,7 +12913,7 @@
       <c r="E167" s="7" t="s">
         <v>739</v>
       </c>
-      <c r="F167" s="8" t="s">
+      <c r="F167" s="61" t="s">
         <v>295</v>
       </c>
       <c r="G167" s="16" t="s">
@@ -12917,7 +12923,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="168" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168" s="3" t="s">
         <v>741</v>
       </c>
@@ -12943,7 +12949,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="169" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A169" s="3" t="s">
         <v>745</v>
       </c>
@@ -12969,7 +12975,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A170" s="3" t="s">
         <v>749</v>
       </c>
@@ -12985,7 +12991,7 @@
       <c r="E170" s="7" t="s">
         <v>751</v>
       </c>
-      <c r="F170" s="8" t="s">
+      <c r="F170" s="61" t="s">
         <v>70</v>
       </c>
       <c r="G170" s="16" t="s">
@@ -12995,7 +13001,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A171" s="18" t="s">
         <v>753</v>
       </c>
@@ -13011,7 +13017,7 @@
       <c r="E171" s="20" t="s">
         <v>755</v>
       </c>
-      <c r="F171" s="21" t="s">
+      <c r="F171" s="62" t="s">
         <v>756</v>
       </c>
       <c r="G171" s="16" t="s">
@@ -13021,7 +13027,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A172" s="18" t="s">
         <v>758</v>
       </c>
@@ -13037,7 +13043,7 @@
       <c r="E172" s="20" t="s">
         <v>760</v>
       </c>
-      <c r="F172" s="21" t="s">
+      <c r="F172" s="62" t="s">
         <v>756</v>
       </c>
       <c r="G172" s="16" t="s">
@@ -13047,7 +13053,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="173" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A173" s="3" t="s">
         <v>762</v>
       </c>
@@ -13073,7 +13079,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="174" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174" s="3" t="s">
         <v>766</v>
       </c>
@@ -13099,7 +13105,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A175" s="18" t="s">
         <v>770</v>
       </c>
@@ -13115,7 +13121,7 @@
       <c r="E175" s="20" t="s">
         <v>772</v>
       </c>
-      <c r="F175" s="21" t="s">
+      <c r="F175" s="62" t="s">
         <v>70</v>
       </c>
       <c r="G175" s="16" t="s">
@@ -13125,7 +13131,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="176" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A176" s="3" t="s">
         <v>774</v>
       </c>
@@ -13151,7 +13157,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="177" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A177" s="3" t="s">
         <v>778</v>
       </c>
@@ -13177,7 +13183,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="178" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A178" s="3" t="s">
         <v>782</v>
       </c>
@@ -13203,7 +13209,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="179" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A179" s="3" t="s">
         <v>786</v>
       </c>
@@ -13229,7 +13235,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="180" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A180" s="3" t="s">
         <v>790</v>
       </c>
@@ -13255,7 +13261,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A181" s="3" t="s">
         <v>794</v>
       </c>
@@ -13271,7 +13277,7 @@
       <c r="E181" s="7" t="s">
         <v>796</v>
       </c>
-      <c r="F181" s="8" t="s">
+      <c r="F181" s="61" t="s">
         <v>39</v>
       </c>
       <c r="G181" s="16" t="s">
@@ -13281,7 +13287,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="182" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A182" s="3" t="s">
         <v>798</v>
       </c>
@@ -13307,7 +13313,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="183" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A183" s="3" t="s">
         <v>802</v>
       </c>
@@ -13333,7 +13339,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="184" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A184" s="3" t="s">
         <v>806</v>
       </c>
@@ -13359,7 +13365,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="185" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A185" s="3" t="s">
         <v>810</v>
       </c>
@@ -13385,7 +13391,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="186" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A186" s="3" t="s">
         <v>814</v>
       </c>
@@ -13411,7 +13417,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="187" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A187" s="3" t="s">
         <v>818</v>
       </c>
@@ -13437,7 +13443,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="188" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A188" s="3" t="s">
         <v>822</v>
       </c>
@@ -13463,7 +13469,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="189" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A189" s="3" t="s">
         <v>826</v>
       </c>
@@ -13489,7 +13495,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="190" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A190" s="3" t="s">
         <v>830</v>
       </c>
@@ -13515,7 +13521,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A191" s="18" t="s">
         <v>834</v>
       </c>
@@ -13531,7 +13537,7 @@
       <c r="E191" s="20" t="s">
         <v>836</v>
       </c>
-      <c r="F191" s="21" t="s">
+      <c r="F191" s="62" t="s">
         <v>70</v>
       </c>
       <c r="G191" s="16" t="s">
@@ -13541,7 +13547,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="192" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A192" s="3" t="s">
         <v>838</v>
       </c>
@@ -13567,7 +13573,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="193" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A193" s="18" t="s">
         <v>843</v>
       </c>
@@ -13593,7 +13599,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A194" s="3" t="s">
         <v>847</v>
       </c>
@@ -13609,7 +13615,7 @@
       <c r="E194" s="7" t="s">
         <v>849</v>
       </c>
-      <c r="F194" s="8" t="s">
+      <c r="F194" s="61" t="s">
         <v>285</v>
       </c>
       <c r="G194" s="16" t="s">
@@ -13619,7 +13625,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="195" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A195" s="3" t="s">
         <v>851</v>
       </c>
@@ -13645,7 +13651,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="196" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A196" s="3" t="s">
         <v>855</v>
       </c>
@@ -13671,7 +13677,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="197" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A197" s="3" t="s">
         <v>859</v>
       </c>
@@ -13697,7 +13703,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A198" s="3" t="s">
         <v>863</v>
       </c>
@@ -13713,7 +13719,7 @@
       <c r="E198" s="7" t="s">
         <v>865</v>
       </c>
-      <c r="F198" s="8" t="s">
+      <c r="F198" s="61" t="s">
         <v>866</v>
       </c>
       <c r="G198" s="16" t="s">
@@ -13723,7 +13729,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="199" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A199" s="3" t="s">
         <v>868</v>
       </c>
@@ -13749,7 +13755,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="200" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A200" s="3" t="s">
         <v>872</v>
       </c>
@@ -13775,7 +13781,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="201" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A201" s="18" t="s">
         <v>876</v>
       </c>
@@ -13801,7 +13807,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="202" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A202" s="3" t="s">
         <v>880</v>
       </c>
@@ -13827,7 +13833,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A203" s="3" t="s">
         <v>885</v>
       </c>
@@ -13843,7 +13849,7 @@
       <c r="E203" s="7" t="s">
         <v>887</v>
       </c>
-      <c r="F203" s="8" t="s">
+      <c r="F203" s="61" t="s">
         <v>271</v>
       </c>
       <c r="G203" s="16" t="s">
@@ -13853,7 +13859,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="204" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A204" s="3" t="s">
         <v>889</v>
       </c>
@@ -13879,7 +13885,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A205" s="3" t="s">
         <v>893</v>
       </c>
@@ -13895,7 +13901,7 @@
       <c r="E205" s="7" t="s">
         <v>895</v>
       </c>
-      <c r="F205" s="8" t="s">
+      <c r="F205" s="61" t="s">
         <v>896</v>
       </c>
       <c r="G205" s="16" t="s">
@@ -13905,7 +13911,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="206" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A206" s="18" t="s">
         <v>898</v>
       </c>
@@ -13931,7 +13937,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A207" s="3" t="s">
         <v>902</v>
       </c>
@@ -13947,7 +13953,7 @@
       <c r="E207" s="7" t="s">
         <v>904</v>
       </c>
-      <c r="F207" s="8" t="s">
+      <c r="F207" s="61" t="s">
         <v>285</v>
       </c>
       <c r="G207" s="16" t="s">
@@ -13957,7 +13963,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="208" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A208" s="3" t="s">
         <v>906</v>
       </c>
@@ -13983,7 +13989,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="209" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A209" s="18" t="s">
         <v>910</v>
       </c>
@@ -14009,7 +14015,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A210" s="3" t="s">
         <v>914</v>
       </c>
@@ -14025,7 +14031,7 @@
       <c r="E210" s="7" t="s">
         <v>916</v>
       </c>
-      <c r="F210" s="8" t="s">
+      <c r="F210" s="61" t="s">
         <v>285</v>
       </c>
       <c r="G210" s="16" t="s">
@@ -14035,7 +14041,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A211" s="3" t="s">
         <v>918</v>
       </c>
@@ -14061,7 +14067,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="212" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A212" s="3" t="s">
         <v>922</v>
       </c>
@@ -14087,7 +14093,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A213" s="3" t="s">
         <v>927</v>
       </c>
@@ -14103,7 +14109,7 @@
       <c r="E213" s="7" t="s">
         <v>929</v>
       </c>
-      <c r="F213" s="8" t="s">
+      <c r="F213" s="61" t="s">
         <v>70</v>
       </c>
       <c r="G213" s="9" t="s">
@@ -14113,7 +14119,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="214" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A214" s="3" t="s">
         <v>931</v>
       </c>
@@ -14139,7 +14145,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="215" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A215" s="3" t="s">
         <v>935</v>
       </c>
@@ -14165,7 +14171,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A216" s="3" t="s">
         <v>939</v>
       </c>
@@ -14181,7 +14187,7 @@
       <c r="E216" s="7" t="s">
         <v>941</v>
       </c>
-      <c r="F216" s="8" t="s">
+      <c r="F216" s="61" t="s">
         <v>295</v>
       </c>
       <c r="G216" s="16" t="s">
@@ -14191,7 +14197,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="217" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A217" s="3" t="s">
         <v>943</v>
       </c>
@@ -14217,7 +14223,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="218" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A218" s="3" t="s">
         <v>947</v>
       </c>
@@ -14243,7 +14249,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A219" s="3" t="s">
         <v>951</v>
       </c>
@@ -14259,7 +14265,7 @@
       <c r="E219" s="7" t="s">
         <v>953</v>
       </c>
-      <c r="F219" s="8" t="s">
+      <c r="F219" s="61" t="s">
         <v>65</v>
       </c>
       <c r="G219" s="16" t="s">
@@ -14269,7 +14275,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="220" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A220" s="3" t="s">
         <v>955</v>
       </c>
@@ -14295,7 +14301,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="221" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A221" s="3" t="s">
         <v>959</v>
       </c>
@@ -14321,7 +14327,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A222" s="3" t="s">
         <v>963</v>
       </c>
@@ -14337,7 +14343,7 @@
       <c r="E222" s="7" t="s">
         <v>965</v>
       </c>
-      <c r="F222" s="8" t="s">
+      <c r="F222" s="61" t="s">
         <v>271</v>
       </c>
       <c r="G222" s="16" t="s">
@@ -14347,7 +14353,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="223" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A223" s="3" t="s">
         <v>967</v>
       </c>
@@ -14373,7 +14379,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="224" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A224" s="3" t="s">
         <v>971</v>
       </c>
@@ -14399,7 +14405,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="225" spans="1:8" ht="145.19999999999999" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:8" ht="140.25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A225" s="3" t="s">
         <v>975</v>
       </c>
@@ -14412,7 +14418,7 @@
       <c r="D225" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E225" s="60" t="s">
+      <c r="E225" s="49" t="s">
         <v>977</v>
       </c>
       <c r="F225" s="8" t="s">
@@ -14425,7 +14431,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="226" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A226" s="3" t="s">
         <v>979</v>
       </c>
@@ -14451,7 +14457,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="227" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A227" s="3" t="s">
         <v>984</v>
       </c>
@@ -14477,7 +14483,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="228" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A228" s="3" t="s">
         <v>988</v>
       </c>
@@ -14503,7 +14509,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="229" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A229" s="3" t="s">
         <v>992</v>
       </c>
@@ -14529,7 +14535,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="230" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A230" s="3" t="s">
         <v>996</v>
       </c>
@@ -14555,7 +14561,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="231" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A231" s="3" t="s">
         <v>1000</v>
       </c>
@@ -14581,7 +14587,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="232" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A232" s="3" t="s">
         <v>1004</v>
       </c>
@@ -14607,7 +14613,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="233" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A233" s="3" t="s">
         <v>1007</v>
       </c>
@@ -14633,7 +14639,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="234" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A234" s="3" t="s">
         <v>1011</v>
       </c>
@@ -14659,7 +14665,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="235" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A235" s="3" t="s">
         <v>1015</v>
       </c>
@@ -14685,7 +14691,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="236" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A236" s="3" t="s">
         <v>1019</v>
       </c>
@@ -14711,7 +14717,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="237" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A237" s="3" t="s">
         <v>1024</v>
       </c>
@@ -14737,7 +14743,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="238" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A238" s="3" t="s">
         <v>1028</v>
       </c>
@@ -14763,7 +14769,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="239" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A239" s="3" t="s">
         <v>1032</v>
       </c>
@@ -14789,7 +14795,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="240" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A240" s="3" t="s">
         <v>1037</v>
       </c>
@@ -14815,7 +14821,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="241" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A241" s="3" t="s">
         <v>1041</v>
       </c>
@@ -14841,7 +14847,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="242" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A242" s="3" t="s">
         <v>1045</v>
       </c>
@@ -14867,7 +14873,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="243" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A243" s="3" t="s">
         <v>1049</v>
       </c>
@@ -14893,7 +14899,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="244" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A244" s="3" t="s">
         <v>1053</v>
       </c>
@@ -14919,7 +14925,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="245" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A245" s="3" t="s">
         <v>1057</v>
       </c>
@@ -14935,7 +14941,7 @@
       <c r="E245" s="7" t="s">
         <v>1059</v>
       </c>
-      <c r="F245" s="8" t="s">
+      <c r="F245" s="61" t="s">
         <v>186</v>
       </c>
       <c r="G245" s="16" t="s">
@@ -14945,7 +14951,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="246" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A246" s="3" t="s">
         <v>1061</v>
       </c>
@@ -14971,7 +14977,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="247" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A247" s="3" t="s">
         <v>1065</v>
       </c>
@@ -14997,7 +15003,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="248" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A248" s="3" t="s">
         <v>1069</v>
       </c>
@@ -15023,7 +15029,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="249" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A249" s="3" t="s">
         <v>1073</v>
       </c>
@@ -15049,7 +15055,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="250" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A250" s="3" t="s">
         <v>1077</v>
       </c>
@@ -15075,7 +15081,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="251" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A251" s="3" t="s">
         <v>1082</v>
       </c>
@@ -15101,7 +15107,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="252" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A252" s="3" t="s">
         <v>1086</v>
       </c>
@@ -15117,7 +15123,7 @@
       <c r="E252" s="7" t="s">
         <v>1088</v>
       </c>
-      <c r="F252" s="8" t="s">
+      <c r="F252" s="61" t="s">
         <v>1089</v>
       </c>
       <c r="G252" s="16" t="s">
@@ -15127,7 +15133,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="253" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A253" s="3" t="s">
         <v>1091</v>
       </c>
@@ -15153,7 +15159,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="254" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A254" s="3" t="s">
         <v>1096</v>
       </c>
@@ -15169,7 +15175,7 @@
       <c r="E254" s="7" t="s">
         <v>1098</v>
       </c>
-      <c r="F254" s="8" t="s">
+      <c r="F254" s="61" t="s">
         <v>295</v>
       </c>
       <c r="G254" s="16" t="s">
@@ -15179,7 +15185,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="255" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A255" s="3" t="s">
         <v>1100</v>
       </c>
@@ -15205,7 +15211,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="256" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A256" s="3" t="s">
         <v>1104</v>
       </c>
@@ -15231,7 +15237,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="257" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A257" s="3" t="s">
         <v>1108</v>
       </c>
@@ -15257,7 +15263,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="258" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A258" s="3" t="s">
         <v>1112</v>
       </c>
@@ -15283,7 +15289,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="259" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A259" s="3" t="s">
         <v>1116</v>
       </c>
@@ -15309,7 +15315,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="260" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A260" s="3" t="s">
         <v>1120</v>
       </c>
@@ -15335,7 +15341,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="261" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A261" s="3" t="s">
         <v>1125</v>
       </c>
@@ -15361,7 +15367,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="262" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A262" s="3" t="s">
         <v>1129</v>
       </c>
@@ -15387,7 +15393,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="263" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A263" s="3" t="s">
         <v>1133</v>
       </c>
@@ -15413,7 +15419,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="264" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A264" s="3" t="s">
         <v>1137</v>
       </c>
@@ -15439,7 +15445,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="265" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A265" s="3" t="s">
         <v>1141</v>
       </c>
@@ -15465,7 +15471,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="266" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A266" s="3" t="s">
         <v>1145</v>
       </c>
@@ -15491,7 +15497,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="267" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A267" s="3" t="s">
         <v>1149</v>
       </c>
@@ -15517,7 +15523,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="268" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A268" s="3" t="s">
         <v>1153</v>
       </c>
@@ -15543,7 +15549,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="269" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A269" s="3" t="s">
         <v>1158</v>
       </c>
@@ -15569,7 +15575,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="270" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A270" s="3" t="s">
         <v>1162</v>
       </c>
@@ -15595,7 +15601,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="271" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A271" s="3" t="s">
         <v>1166</v>
       </c>
@@ -15611,7 +15617,7 @@
       <c r="E271" s="7" t="s">
         <v>1167</v>
       </c>
-      <c r="F271" s="8" t="s">
+      <c r="F271" s="61" t="s">
         <v>1164</v>
       </c>
       <c r="G271" s="16" t="s">
@@ -15621,7 +15627,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="272" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A272" s="3" t="s">
         <v>1169</v>
       </c>
@@ -15647,7 +15653,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="273" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A273" s="3" t="s">
         <v>1174</v>
       </c>
@@ -15673,7 +15679,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="274" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A274" s="3" t="s">
         <v>1178</v>
       </c>
@@ -15699,7 +15705,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="275" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A275" s="3" t="s">
         <v>1182</v>
       </c>
@@ -15725,7 +15731,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="276" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A276" s="3" t="s">
         <v>1186</v>
       </c>
@@ -15751,7 +15757,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="277" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A277" s="3" t="s">
         <v>1190</v>
       </c>
@@ -15777,7 +15783,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="278" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A278" s="3" t="s">
         <v>1194</v>
       </c>
@@ -15803,7 +15809,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="279" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A279" s="3" t="s">
         <v>1198</v>
       </c>
@@ -15829,7 +15835,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="280" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A280" s="3" t="s">
         <v>1201</v>
       </c>
@@ -15855,7 +15861,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="281" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A281" s="3" t="s">
         <v>1205</v>
       </c>
@@ -15881,7 +15887,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="282" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A282" s="3" t="s">
         <v>1209</v>
       </c>
@@ -15907,7 +15913,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="283" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A283" s="3" t="s">
         <v>1213</v>
       </c>
@@ -15933,7 +15939,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="284" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A284" s="3" t="s">
         <v>1217</v>
       </c>
@@ -15959,7 +15965,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="285" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A285" s="3" t="s">
         <v>1221</v>
       </c>
@@ -15985,7 +15991,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="286" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A286" s="3" t="s">
         <v>1225</v>
       </c>
@@ -16011,7 +16017,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="287" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A287" s="3" t="s">
         <v>1228</v>
       </c>
@@ -16037,7 +16043,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="288" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A288" s="3" t="s">
         <v>1233</v>
       </c>
@@ -16063,7 +16069,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="289" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A289" s="3" t="s">
         <v>1237</v>
       </c>
@@ -16089,7 +16095,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="290" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A290" s="3" t="s">
         <v>1241</v>
       </c>
@@ -16115,7 +16121,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="291" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A291" s="18" t="s">
         <v>1245</v>
       </c>
@@ -16141,7 +16147,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="292" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A292" s="3" t="s">
         <v>1249</v>
       </c>
@@ -16167,7 +16173,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="293" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A293" s="3" t="s">
         <v>1253</v>
       </c>
@@ -16193,7 +16199,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="294" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A294" s="3" t="s">
         <v>1257</v>
       </c>
@@ -16219,7 +16225,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="295" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A295" s="3" t="s">
         <v>1261</v>
       </c>
@@ -16245,7 +16251,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="296" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A296" s="3" t="s">
         <v>1264</v>
       </c>
@@ -16271,7 +16277,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="297" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A297" s="3" t="s">
         <v>1268</v>
       </c>
@@ -16297,7 +16303,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="298" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A298" s="3" t="s">
         <v>1272</v>
       </c>
@@ -16323,7 +16329,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="299" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A299" s="3" t="s">
         <v>1276</v>
       </c>
@@ -16349,7 +16355,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="300" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A300" s="3" t="s">
         <v>1280</v>
       </c>
@@ -16375,7 +16381,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="301" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A301" s="3" t="s">
         <v>1284</v>
       </c>
@@ -16401,7 +16407,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="302" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:8" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A302" s="3" t="s">
         <v>1288</v>
       </c>
@@ -16432,7 +16438,6 @@
     <filterColumn colId="3">
       <filters>
         <filter val="Fácil"/>
-        <filter val="Insane"/>
       </filters>
     </filterColumn>
     <filterColumn colId="5">
@@ -16462,11 +16467,16 @@
         <filter val="OSCP_x000a_OSEP_x000a_eCPPTv3_x000a_Active Directory"/>
       </filters>
     </filterColumn>
+    <filterColumn colId="7">
+      <filters>
+        <filter val="No"/>
+      </filters>
+    </filterColumn>
   </autoFilter>
   <customSheetViews>
     <customSheetView guid="{9FAF8FF3-7EC5-4D1C-B7E7-3FED51CA7755}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A4:H27" xr:uid="{F6CE6A65-482E-4620-8A85-82AACC25B82A}"/>
+      <autoFilter ref="A4:H27" xr:uid="{E859BE4E-AABC-48A0-A2A4-2E7B3FE5BEF0}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="1">
@@ -16786,17 +16796,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
-    <col min="3" max="3" width="62.33203125" customWidth="1"/>
-    <col min="4" max="4" width="46.6640625" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="62.28515625" customWidth="1"/>
+    <col min="4" max="4" width="46.7109375" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="12.77734375" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
         <v>1292</v>
       </c>
@@ -16805,7 +16815,7 @@
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>1293</v>
       </c>
@@ -16825,7 +16835,7 @@
       <c r="G4" s="29"/>
       <c r="H4" s="29"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="30" t="s">
         <v>1296</v>
       </c>
@@ -16842,7 +16852,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="30" t="s">
         <v>1301</v>
       </c>
@@ -16859,7 +16869,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="30" t="s">
         <v>1305</v>
       </c>
@@ -16876,7 +16886,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="30" t="s">
         <v>1308</v>
       </c>
@@ -16893,7 +16903,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>1311</v>
       </c>
@@ -16910,7 +16920,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="30" t="s">
         <v>1314</v>
       </c>
@@ -16927,7 +16937,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>1318</v>
       </c>
@@ -16944,7 +16954,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>1321</v>
       </c>
@@ -16961,7 +16971,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>1324</v>
       </c>
@@ -16978,7 +16988,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>1328</v>
       </c>
@@ -16995,7 +17005,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>1331</v>
       </c>
@@ -17012,7 +17022,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>1334</v>
       </c>
@@ -17029,7 +17039,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>1337</v>
       </c>
@@ -17076,18 +17086,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.44140625" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" customWidth="1"/>
-    <col min="4" max="4" width="99.21875" customWidth="1"/>
-    <col min="5" max="5" width="16.77734375" customWidth="1"/>
-    <col min="6" max="6" width="53.21875" customWidth="1"/>
-    <col min="7" max="7" width="43.21875" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="99.28515625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="53.28515625" customWidth="1"/>
+    <col min="7" max="7" width="43.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -17113,7 +17123,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>1341</v>
       </c>
@@ -17139,7 +17149,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>1345</v>
       </c>
@@ -17165,7 +17175,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>1350</v>
       </c>
@@ -17191,7 +17201,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>1355</v>
       </c>
@@ -17217,7 +17227,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>1358</v>
       </c>
@@ -17243,7 +17253,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>1362</v>
       </c>
@@ -17269,7 +17279,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>1365</v>
       </c>
@@ -17295,7 +17305,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>1370</v>
       </c>
@@ -17321,7 +17331,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>1374</v>
       </c>
@@ -17347,7 +17357,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>1378</v>
       </c>
@@ -17373,7 +17383,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="18" t="s">
         <v>1383</v>
       </c>
@@ -17399,7 +17409,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="18" t="s">
         <v>1387</v>
       </c>
@@ -17425,7 +17435,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="18" t="s">
         <v>1391</v>
       </c>
@@ -17451,7 +17461,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="18" t="s">
         <v>1395</v>
       </c>
@@ -17477,7 +17487,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="18" t="s">
         <v>1399</v>
       </c>
@@ -17503,7 +17513,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="18" t="s">
         <v>1403</v>
       </c>
@@ -17529,7 +17539,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="18" t="s">
         <v>1406</v>
       </c>
@@ -17555,7 +17565,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="18" t="s">
         <v>321</v>
       </c>
@@ -17581,7 +17591,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="18" t="s">
         <v>1413</v>
       </c>
@@ -17607,7 +17617,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="18" t="s">
         <v>1416</v>
       </c>
@@ -17633,7 +17643,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="18" t="s">
         <v>1420</v>
       </c>
@@ -17659,7 +17669,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="18" t="s">
         <v>1424</v>
       </c>
@@ -17685,7 +17695,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="18" t="s">
         <v>1427</v>
       </c>
@@ -17711,7 +17721,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="18" t="s">
         <v>1431</v>
       </c>
@@ -17737,7 +17747,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="18" t="s">
         <v>1436</v>
       </c>
@@ -17763,7 +17773,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="18" t="s">
         <v>1440</v>
       </c>
@@ -17789,7 +17799,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="18" t="s">
         <v>1444</v>
       </c>
@@ -17815,7 +17825,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="18" t="s">
         <v>1447</v>
       </c>
@@ -17841,7 +17851,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="18" t="s">
         <v>1451</v>
       </c>
@@ -17867,7 +17877,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="18" t="s">
         <v>1455</v>
       </c>
@@ -17893,7 +17903,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="18" t="s">
         <v>1459</v>
       </c>
@@ -17919,7 +17929,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="18" t="s">
         <v>1463</v>
       </c>
@@ -17945,7 +17955,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="18" t="s">
         <v>1467</v>
       </c>
@@ -17971,7 +17981,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="18" t="s">
         <v>1471</v>
       </c>
@@ -17997,7 +18007,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="18" t="s">
         <v>1475</v>
       </c>
@@ -18023,7 +18033,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="18" t="s">
         <v>1479</v>
       </c>
@@ -18049,7 +18059,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="18" t="s">
         <v>1483</v>
       </c>
@@ -18075,7 +18085,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="18" t="s">
         <v>1487</v>
       </c>
@@ -18101,7 +18111,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="18" t="s">
         <v>1491</v>
       </c>
@@ -18127,7 +18137,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="18" t="s">
         <v>1495</v>
       </c>
@@ -18153,7 +18163,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>1499</v>
       </c>
@@ -18179,7 +18189,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>1503</v>
       </c>
@@ -18205,7 +18215,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="18" t="s">
         <v>1507</v>
       </c>
@@ -18231,7 +18241,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="18" t="s">
         <v>1512</v>
       </c>
@@ -18257,7 +18267,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="18" t="s">
         <v>1516</v>
       </c>
@@ -18283,7 +18293,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>1520</v>
       </c>
@@ -18309,7 +18319,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>1523</v>
       </c>
@@ -18335,7 +18345,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>1527</v>
       </c>
@@ -18361,7 +18371,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>1531</v>
       </c>
@@ -18387,7 +18397,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>1536</v>
       </c>
@@ -18413,7 +18423,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>1540</v>
       </c>
@@ -18439,7 +18449,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>1544</v>
       </c>
@@ -18465,7 +18475,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>1548</v>
       </c>
@@ -18491,7 +18501,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>1552</v>
       </c>
@@ -18517,7 +18527,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>1556</v>
       </c>
@@ -18543,7 +18553,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>1560</v>
       </c>
@@ -18569,7 +18579,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>1563</v>
       </c>
@@ -18595,7 +18605,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>1567</v>
       </c>
@@ -18764,15 +18774,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.77734375" customWidth="1"/>
-    <col min="2" max="2" width="72.109375" customWidth="1"/>
-    <col min="3" max="3" width="43.109375" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" customWidth="1"/>
+    <col min="1" max="1" width="32.7109375" customWidth="1"/>
+    <col min="2" max="2" width="72.140625" customWidth="1"/>
+    <col min="3" max="3" width="43.140625" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1571</v>
       </c>
@@ -18789,382 +18799,389 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="52" t="s">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="57" t="s">
         <v>1573</v>
       </c>
       <c r="B3" s="45" t="s">
         <v>1574</v>
       </c>
-      <c r="C3" s="55" t="s">
+      <c r="C3" s="58" t="s">
         <v>1575</v>
       </c>
-      <c r="D3" s="56" t="s">
+      <c r="D3" s="53" t="s">
         <v>204</v>
       </c>
-      <c r="E3" s="57" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="53"/>
+      <c r="E3" s="56" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="54"/>
       <c r="B4" s="45" t="s">
         <v>1576</v>
       </c>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="53"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="54"/>
       <c r="B5" s="46" t="s">
         <v>1577</v>
       </c>
-      <c r="C5" s="53"/>
-      <c r="D5" s="53"/>
-      <c r="E5" s="53"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="53"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="54"/>
       <c r="B6" s="46" t="s">
         <v>1578</v>
       </c>
-      <c r="C6" s="53"/>
-      <c r="D6" s="53"/>
-      <c r="E6" s="53"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="53"/>
+      <c r="C6" s="54"/>
+      <c r="D6" s="54"/>
+      <c r="E6" s="54"/>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="54"/>
       <c r="B7" s="46" t="s">
         <v>1579</v>
       </c>
-      <c r="C7" s="53"/>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="53"/>
+      <c r="C7" s="54"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="54"/>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="54"/>
       <c r="B8" s="46" t="s">
         <v>1580</v>
       </c>
-      <c r="C8" s="53"/>
-      <c r="D8" s="53"/>
-      <c r="E8" s="53"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="53"/>
+      <c r="C8" s="54"/>
+      <c r="D8" s="54"/>
+      <c r="E8" s="54"/>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="54"/>
       <c r="B9" s="46" t="s">
         <v>1581</v>
       </c>
-      <c r="C9" s="53"/>
-      <c r="D9" s="53"/>
-      <c r="E9" s="53"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="53"/>
+      <c r="C9" s="54"/>
+      <c r="D9" s="54"/>
+      <c r="E9" s="54"/>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="54"/>
       <c r="B10" s="46" t="s">
         <v>1582</v>
       </c>
-      <c r="C10" s="53"/>
-      <c r="D10" s="53"/>
-      <c r="E10" s="53"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="53"/>
+      <c r="C10" s="54"/>
+      <c r="D10" s="54"/>
+      <c r="E10" s="54"/>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="54"/>
       <c r="B11" s="46" t="s">
         <v>1583</v>
       </c>
-      <c r="C11" s="53"/>
-      <c r="D11" s="53"/>
-      <c r="E11" s="53"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="53"/>
+      <c r="C11" s="54"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="54"/>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="54"/>
       <c r="B12" s="46" t="s">
         <v>1584</v>
       </c>
-      <c r="C12" s="53"/>
-      <c r="D12" s="53"/>
-      <c r="E12" s="53"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="53"/>
+      <c r="C12" s="54"/>
+      <c r="D12" s="54"/>
+      <c r="E12" s="54"/>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="54"/>
       <c r="B13" s="46" t="s">
         <v>1585</v>
       </c>
-      <c r="C13" s="53"/>
-      <c r="D13" s="53"/>
-      <c r="E13" s="53"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="53"/>
+      <c r="C13" s="54"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="54"/>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="54"/>
       <c r="B14" s="46" t="s">
         <v>1586</v>
       </c>
-      <c r="C14" s="53"/>
-      <c r="D14" s="53"/>
-      <c r="E14" s="53"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="53"/>
+      <c r="C14" s="54"/>
+      <c r="D14" s="54"/>
+      <c r="E14" s="54"/>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="54"/>
       <c r="B15" s="46" t="s">
         <v>1587</v>
       </c>
-      <c r="C15" s="53"/>
-      <c r="D15" s="53"/>
-      <c r="E15" s="53"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="53"/>
+      <c r="C15" s="54"/>
+      <c r="D15" s="54"/>
+      <c r="E15" s="54"/>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="54"/>
       <c r="B16" s="46" t="s">
         <v>1588</v>
       </c>
-      <c r="C16" s="53"/>
-      <c r="D16" s="53"/>
-      <c r="E16" s="53"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="53"/>
+      <c r="C16" s="54"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="54"/>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="54"/>
       <c r="B17" s="46" t="s">
         <v>1589</v>
       </c>
-      <c r="C17" s="53"/>
-      <c r="D17" s="53"/>
-      <c r="E17" s="53"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="53"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="54"/>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="54"/>
       <c r="B18" s="46" t="s">
         <v>1590</v>
       </c>
-      <c r="C18" s="53"/>
-      <c r="D18" s="53"/>
-      <c r="E18" s="53"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="54"/>
+      <c r="C18" s="54"/>
+      <c r="D18" s="54"/>
+      <c r="E18" s="54"/>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="55"/>
       <c r="B19" s="45" t="s">
         <v>1591</v>
       </c>
-      <c r="C19" s="54"/>
-      <c r="D19" s="54"/>
-      <c r="E19" s="54"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="52" t="s">
+      <c r="C19" s="55"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="55"/>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="57" t="s">
         <v>1592</v>
       </c>
       <c r="B20" s="47" t="s">
         <v>1593</v>
       </c>
-      <c r="C20" s="55" t="s">
+      <c r="C20" s="58" t="s">
         <v>1594</v>
       </c>
-      <c r="D20" s="56" t="s">
+      <c r="D20" s="53" t="s">
         <v>204</v>
       </c>
-      <c r="E20" s="57" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="53"/>
+      <c r="E20" s="56" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="54"/>
       <c r="B21" s="47" t="s">
         <v>1595</v>
       </c>
-      <c r="C21" s="53"/>
-      <c r="D21" s="53"/>
-      <c r="E21" s="53"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="53"/>
+      <c r="C21" s="54"/>
+      <c r="D21" s="54"/>
+      <c r="E21" s="54"/>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="54"/>
       <c r="B22" s="47" t="s">
         <v>1596</v>
       </c>
-      <c r="C22" s="53"/>
-      <c r="D22" s="53"/>
-      <c r="E22" s="53"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="53"/>
+      <c r="C22" s="54"/>
+      <c r="D22" s="54"/>
+      <c r="E22" s="54"/>
+    </row>
+    <row r="23" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A23" s="54"/>
       <c r="B23" s="47" t="s">
         <v>1597</v>
       </c>
-      <c r="C23" s="53"/>
-      <c r="D23" s="53"/>
-      <c r="E23" s="53"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="53"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="54"/>
+    </row>
+    <row r="24" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="54"/>
       <c r="B24" s="47" t="s">
         <v>1598</v>
       </c>
-      <c r="C24" s="53"/>
-      <c r="D24" s="53"/>
-      <c r="E24" s="53"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="53"/>
+      <c r="C24" s="54"/>
+      <c r="D24" s="54"/>
+      <c r="E24" s="54"/>
+    </row>
+    <row r="25" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="54"/>
       <c r="B25" s="47" t="s">
         <v>1599</v>
       </c>
-      <c r="C25" s="53"/>
-      <c r="D25" s="53"/>
-      <c r="E25" s="53"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="53"/>
+      <c r="C25" s="54"/>
+      <c r="D25" s="54"/>
+      <c r="E25" s="54"/>
+    </row>
+    <row r="26" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A26" s="54"/>
       <c r="B26" s="47" t="s">
         <v>1600</v>
       </c>
-      <c r="C26" s="53"/>
-      <c r="D26" s="53"/>
-      <c r="E26" s="53"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="54"/>
+      <c r="C26" s="54"/>
+      <c r="D26" s="54"/>
+      <c r="E26" s="54"/>
+    </row>
+    <row r="27" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A27" s="55"/>
       <c r="B27" s="47" t="s">
         <v>1601</v>
       </c>
-      <c r="C27" s="54"/>
-      <c r="D27" s="54"/>
-      <c r="E27" s="54"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="52" t="s">
+      <c r="C27" s="55"/>
+      <c r="D27" s="55"/>
+      <c r="E27" s="55"/>
+    </row>
+    <row r="28" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A28" s="57" t="s">
         <v>1602</v>
       </c>
       <c r="B28" s="47" t="s">
         <v>1603</v>
       </c>
-      <c r="C28" s="55" t="s">
+      <c r="C28" s="58" t="s">
         <v>1604</v>
       </c>
-      <c r="D28" s="56" t="s">
+      <c r="D28" s="53" t="s">
         <v>121</v>
       </c>
-      <c r="E28" s="57" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="53"/>
+      <c r="E28" s="56" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A29" s="54"/>
       <c r="B29" s="47" t="s">
         <v>1605</v>
       </c>
-      <c r="C29" s="53"/>
-      <c r="D29" s="53"/>
-      <c r="E29" s="53"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="53"/>
+      <c r="C29" s="54"/>
+      <c r="D29" s="54"/>
+      <c r="E29" s="54"/>
+    </row>
+    <row r="30" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A30" s="54"/>
       <c r="B30" s="47" t="s">
         <v>1606</v>
       </c>
-      <c r="C30" s="53"/>
-      <c r="D30" s="53"/>
-      <c r="E30" s="53"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="53"/>
+      <c r="C30" s="54"/>
+      <c r="D30" s="54"/>
+      <c r="E30" s="54"/>
+    </row>
+    <row r="31" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A31" s="54"/>
       <c r="B31" s="47" t="s">
         <v>1607</v>
       </c>
-      <c r="C31" s="53"/>
-      <c r="D31" s="53"/>
-      <c r="E31" s="53"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="53"/>
+      <c r="C31" s="54"/>
+      <c r="D31" s="54"/>
+      <c r="E31" s="54"/>
+    </row>
+    <row r="32" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A32" s="54"/>
       <c r="B32" s="47" t="s">
         <v>1608</v>
       </c>
-      <c r="C32" s="53"/>
-      <c r="D32" s="53"/>
-      <c r="E32" s="53"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="54"/>
+      <c r="C32" s="54"/>
+      <c r="D32" s="54"/>
+      <c r="E32" s="54"/>
+    </row>
+    <row r="33" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A33" s="55"/>
       <c r="B33" s="47" t="s">
         <v>1609</v>
       </c>
-      <c r="C33" s="54"/>
-      <c r="D33" s="54"/>
-      <c r="E33" s="54"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="52" t="s">
+      <c r="C33" s="55"/>
+      <c r="D33" s="55"/>
+      <c r="E33" s="55"/>
+    </row>
+    <row r="34" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A34" s="57" t="s">
         <v>1610</v>
       </c>
       <c r="B34" s="47" t="s">
         <v>1611</v>
       </c>
-      <c r="C34" s="55" t="s">
+      <c r="C34" s="58" t="s">
         <v>1612</v>
       </c>
-      <c r="D34" s="56" t="s">
+      <c r="D34" s="53" t="s">
         <v>204</v>
       </c>
-      <c r="E34" s="57" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="53"/>
+      <c r="E34" s="56" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A35" s="54"/>
       <c r="B35" s="47" t="s">
         <v>1613</v>
       </c>
-      <c r="C35" s="53"/>
-      <c r="D35" s="53"/>
-      <c r="E35" s="53"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="53"/>
+      <c r="C35" s="54"/>
+      <c r="D35" s="54"/>
+      <c r="E35" s="54"/>
+    </row>
+    <row r="36" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A36" s="54"/>
       <c r="B36" s="47" t="s">
         <v>1614</v>
       </c>
-      <c r="C36" s="53"/>
-      <c r="D36" s="53"/>
-      <c r="E36" s="53"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="53"/>
+      <c r="C36" s="54"/>
+      <c r="D36" s="54"/>
+      <c r="E36" s="54"/>
+    </row>
+    <row r="37" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A37" s="54"/>
       <c r="B37" s="47" t="s">
         <v>1615</v>
       </c>
-      <c r="C37" s="53"/>
-      <c r="D37" s="53"/>
-      <c r="E37" s="53"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="53"/>
+      <c r="C37" s="54"/>
+      <c r="D37" s="54"/>
+      <c r="E37" s="54"/>
+    </row>
+    <row r="38" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A38" s="54"/>
       <c r="B38" s="47" t="s">
         <v>1616</v>
       </c>
-      <c r="C38" s="53"/>
-      <c r="D38" s="53"/>
-      <c r="E38" s="53"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="53"/>
+      <c r="C38" s="54"/>
+      <c r="D38" s="54"/>
+      <c r="E38" s="54"/>
+    </row>
+    <row r="39" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A39" s="54"/>
       <c r="B39" s="47" t="s">
         <v>1617</v>
       </c>
-      <c r="C39" s="53"/>
-      <c r="D39" s="53"/>
-      <c r="E39" s="53"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="54"/>
+      <c r="C39" s="54"/>
+      <c r="D39" s="54"/>
+      <c r="E39" s="54"/>
+    </row>
+    <row r="40" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A40" s="55"/>
       <c r="B40" s="47" t="s">
         <v>1618</v>
       </c>
-      <c r="C40" s="54"/>
-      <c r="D40" s="54"/>
-      <c r="E40" s="54"/>
+      <c r="C40" s="55"/>
+      <c r="D40" s="55"/>
+      <c r="E40" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A3:A19"/>
+    <mergeCell ref="C3:C19"/>
+    <mergeCell ref="D3:D19"/>
+    <mergeCell ref="E3:E19"/>
+    <mergeCell ref="C20:C27"/>
+    <mergeCell ref="D20:D27"/>
+    <mergeCell ref="E20:E27"/>
     <mergeCell ref="D34:D40"/>
     <mergeCell ref="E34:E40"/>
     <mergeCell ref="A20:A27"/>
@@ -19174,13 +19191,6 @@
     <mergeCell ref="E28:E33"/>
     <mergeCell ref="A34:A40"/>
     <mergeCell ref="C34:C40"/>
-    <mergeCell ref="A3:A19"/>
-    <mergeCell ref="C3:C19"/>
-    <mergeCell ref="D3:D19"/>
-    <mergeCell ref="E3:E19"/>
-    <mergeCell ref="C20:C27"/>
-    <mergeCell ref="D20:D27"/>
-    <mergeCell ref="E20:E27"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" sqref="E3 E20 E28 E34" xr:uid="{00000000-0002-0000-0300-000000000000}">
@@ -19244,26 +19254,26 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.21875" customWidth="1"/>
-    <col min="4" max="4" width="58.77734375" customWidth="1"/>
-    <col min="5" max="5" width="14.77734375" customWidth="1"/>
-    <col min="6" max="6" width="55.77734375" customWidth="1"/>
-    <col min="7" max="7" width="19.77734375" customWidth="1"/>
-    <col min="8" max="8" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="4" max="4" width="58.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1"/>
+    <col min="6" max="6" width="55.7109375" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" customWidth="1"/>
+    <col min="8" max="8" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="59" t="s">
         <v>1619</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
       <c r="E1" s="28"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -19292,7 +19302,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>1622</v>
       </c>

</xml_diff>